<commit_message>
more hts forms cleanup
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_linkage.xlsx
+++ b/config/default/forms/app/hts_linkage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="171">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kemr_uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMR Client Reference</t>
   </si>
   <si>
     <t xml:space="preserve">db:person</t>
@@ -540,7 +546,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -575,6 +581,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -719,7 +739,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -740,7 +760,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -748,15 +780,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,39 +796,39 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,11 +836,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1409,32 +1441,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y65536"/>
+  <dimension ref="A1:AL65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="13:13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.1173469387755"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="76.765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="90.984693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.4642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="94.3163265306123"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="37.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,54 +1834,65 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7"/>
+      <c r="AL13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1872,17 +1915,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1905,10 +1950,14 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -1934,14 +1983,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
@@ -1970,14 +2015,14 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -2003,10 +2048,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2033,13 +2078,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2069,7 +2114,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>43</v>
@@ -2099,10 +2144,14 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2159,8 +2208,8 @@
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2244,22 +2293,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -2279,10 +2322,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
@@ -2293,7 +2336,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2313,218 +2356,218 @@
       <c r="Y28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>47</v>
+      <c r="A29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="6" t="s">
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>59</v>
@@ -2537,7 +2580,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="9" t="s">
         <v>60</v>
       </c>
       <c r="J35" s="4"/>
@@ -2557,800 +2600,800 @@
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="5" t="s">
+    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5" t="s">
+      <c r="C37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
-      <c r="V36" s="5"/>
-      <c r="W36" s="5"/>
-      <c r="X36" s="5"/>
-      <c r="Y36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="D37" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="D38" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5" t="s">
+      <c r="B39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
-      <c r="Y38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="B40" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5" t="s">
+      <c r="C40" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="D40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
-      <c r="Y40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="4" t="s">
+      <c r="D41" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="C42" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
-      <c r="Y41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="D42" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="H42" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
-      <c r="X43" s="5"/>
-      <c r="Y43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
-      <c r="Y44" s="5"/>
-    </row>
-    <row r="45" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="B44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C44" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="9" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
-      <c r="Y45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
-      <c r="Y46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="D46" s="8"/>
+      <c r="E46" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="4" t="s">
+      <c r="F46" s="8"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="C48" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="D48" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="H48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H48" s="4" t="s">
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
-      <c r="Y48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="C49" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
-      <c r="Y49" s="5"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="8"/>
+      <c r="X49" s="8"/>
+      <c r="Y49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
+      <c r="A50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
-      <c r="Y50" s="5"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+      <c r="Y50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="5"/>
-      <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
-      <c r="W51" s="5"/>
-      <c r="X51" s="5"/>
-      <c r="Y51" s="5"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
+      <c r="Y51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="5"/>
-      <c r="X52" s="5"/>
-      <c r="Y52" s="5"/>
-    </row>
-    <row r="53" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+      <c r="X53" s="8"/>
+      <c r="Y53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F53" s="5" t="s">
+      <c r="B54" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="5"/>
-      <c r="X53" s="5"/>
-      <c r="Y53" s="5"/>
-    </row>
-    <row r="54" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="D54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
-      <c r="W54" s="5"/>
-      <c r="X54" s="5"/>
-      <c r="Y54" s="5"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="8"/>
+      <c r="X54" s="8"/>
+      <c r="Y54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5" t="s">
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="8"/>
+      <c r="W55" s="8"/>
+      <c r="X55" s="8"/>
+      <c r="Y55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
-      <c r="V55" s="5"/>
-      <c r="W55" s="5"/>
-      <c r="X55" s="5"/>
-      <c r="Y55" s="5"/>
-    </row>
-    <row r="56" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
-      <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
-      <c r="Y56" s="5"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="8"/>
+      <c r="X56" s="8"/>
+      <c r="Y56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5" t="s">
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="8"/>
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
+      <c r="V57" s="8"/>
+      <c r="W57" s="8"/>
+      <c r="X57" s="8"/>
+      <c r="Y57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5"/>
-      <c r="T57" s="5"/>
-      <c r="U57" s="5"/>
-      <c r="V57" s="5"/>
-      <c r="W57" s="5"/>
-      <c r="X57" s="5"/>
-      <c r="Y57" s="5"/>
-    </row>
-    <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B58" s="10" t="s">
+      <c r="C58" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
-      <c r="X58" s="4"/>
-      <c r="Y58" s="4"/>
-    </row>
-    <row r="59" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="4" t="s">
         <v>118</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -3371,386 +3414,397 @@
       <c r="X59" s="4"/>
       <c r="Y59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" s="5" t="s">
+    <row r="60" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
-      <c r="V61" s="4"/>
-      <c r="W61" s="4"/>
-      <c r="X61" s="4"/>
-      <c r="Y61" s="4"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="8"/>
+      <c r="X61" s="8"/>
+      <c r="Y61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" s="5" t="s">
+      <c r="A62" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="5"/>
-      <c r="U62" s="5"/>
-      <c r="V62" s="5"/>
-      <c r="W62" s="5"/>
-      <c r="X62" s="5"/>
-      <c r="Y62" s="5"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="11" t="s">
+      <c r="A63" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-      <c r="U63" s="4"/>
-      <c r="V63" s="4"/>
-      <c r="W63" s="4"/>
-      <c r="X63" s="4"/>
-      <c r="Y63" s="4"/>
-    </row>
-    <row r="64" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="5" t="s">
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+      <c r="Y63" s="8"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="4" t="s">
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="4"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+    </row>
+    <row r="65" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D65" s="8"/>
+      <c r="E65" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-      <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="5"/>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
+      <c r="F65" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+      <c r="R65" s="8"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="8"/>
+      <c r="X65" s="8"/>
+      <c r="Y65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="11" t="s">
+      <c r="A66" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
-      <c r="V66" s="4"/>
-      <c r="W66" s="4"/>
-      <c r="X66" s="4"/>
-      <c r="Y66" s="4"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="8"/>
+      <c r="N66" s="8"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="8"/>
+      <c r="R66" s="8"/>
+      <c r="S66" s="8"/>
+      <c r="T66" s="8"/>
+      <c r="U66" s="8"/>
+      <c r="V66" s="8"/>
+      <c r="W66" s="8"/>
+      <c r="X66" s="8"/>
+      <c r="Y66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B67" s="5" t="s">
+      <c r="A67" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5"/>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
-      <c r="U67" s="5"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="5"/>
-      <c r="X67" s="5"/>
-      <c r="Y67" s="5"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
+      <c r="X67" s="4"/>
+      <c r="Y67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B68" s="11" t="s">
+      <c r="A68" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
-      <c r="U68" s="4"/>
-      <c r="V68" s="4"/>
-      <c r="W68" s="4"/>
-      <c r="X68" s="4"/>
-      <c r="Y68" s="4"/>
-    </row>
-    <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+      <c r="T68" s="8"/>
+      <c r="U68" s="8"/>
+      <c r="V68" s="8"/>
+      <c r="W68" s="8"/>
+      <c r="X68" s="8"/>
+      <c r="Y68" s="8"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="4"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="12" t="s">
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
+      <c r="P70" s="8"/>
+      <c r="Q70" s="8"/>
+      <c r="R70" s="8"/>
+      <c r="S70" s="8"/>
+      <c r="T70" s="8"/>
+      <c r="U70" s="8"/>
+      <c r="V70" s="8"/>
+      <c r="W70" s="8"/>
+      <c r="X70" s="8"/>
+      <c r="Y70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C70" s="12" t="s">
+      <c r="B71" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="12" t="s">
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-    </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
       <c r="G71" s="16"/>
       <c r="H71" s="16"/>
-      <c r="I71" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="I71" s="16"/>
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
       <c r="L71" s="16"/>
@@ -3759,106 +3813,103 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J72" s="19"/>
+      <c r="K72" s="19"/>
+      <c r="L72" s="19"/>
+      <c r="M72" s="19"/>
+      <c r="N72" s="19"/>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
-      <c r="Y73" s="5"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="M73" s="16"/>
+      <c r="N73" s="16"/>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-      <c r="P74" s="5"/>
-      <c r="Q74" s="5"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="5"/>
-      <c r="W74" s="5"/>
-      <c r="X74" s="5"/>
-      <c r="Y74" s="5"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="8"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="8"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="8"/>
+      <c r="V74" s="8"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-      <c r="Q75" s="4"/>
-      <c r="R75" s="4"/>
-      <c r="S75" s="4"/>
-      <c r="T75" s="4"/>
-      <c r="U75" s="4"/>
-      <c r="V75" s="4"/>
-      <c r="W75" s="4"/>
-      <c r="X75" s="4"/>
-      <c r="Y75" s="4"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="8"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="8"/>
+      <c r="Q75" s="8"/>
+      <c r="R75" s="8"/>
+      <c r="S75" s="8"/>
+      <c r="T75" s="8"/>
+      <c r="U75" s="8"/>
+      <c r="V75" s="8"/>
+      <c r="W75" s="8"/>
+      <c r="X75" s="8"/>
+      <c r="Y75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3965,330 +4016,356 @@
       <c r="Y79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="5"/>
-      <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
-      <c r="W80" s="5"/>
-      <c r="X80" s="5"/>
-      <c r="Y80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
+      <c r="X80" s="4"/>
+      <c r="Y80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
-      <c r="U81" s="4"/>
-      <c r="V81" s="4"/>
-      <c r="W81" s="4"/>
-      <c r="X81" s="4"/>
-      <c r="Y81" s="4"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="8"/>
+      <c r="Q81" s="8"/>
+      <c r="R81" s="8"/>
+      <c r="S81" s="8"/>
+      <c r="T81" s="8"/>
+      <c r="U81" s="8"/>
+      <c r="V81" s="8"/>
+      <c r="W81" s="8"/>
+      <c r="X81" s="8"/>
+      <c r="Y81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5"/>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
-      <c r="Y82" s="5"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="4"/>
+      <c r="S82" s="4"/>
+      <c r="T82" s="4"/>
+      <c r="U82" s="4"/>
+      <c r="V82" s="4"/>
+      <c r="W82" s="4"/>
+      <c r="X82" s="4"/>
+      <c r="Y82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
-      <c r="R83" s="5"/>
-      <c r="S83" s="5"/>
-      <c r="T83" s="5"/>
-      <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
-      <c r="W83" s="5"/>
-      <c r="X83" s="5"/>
-      <c r="Y83" s="5"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="8"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="8"/>
+      <c r="Q83" s="8"/>
+      <c r="R83" s="8"/>
+      <c r="S83" s="8"/>
+      <c r="T83" s="8"/>
+      <c r="U83" s="8"/>
+      <c r="V83" s="8"/>
+      <c r="W83" s="8"/>
+      <c r="X83" s="8"/>
+      <c r="Y83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-      <c r="P84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="R84" s="5"/>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="5"/>
-      <c r="V84" s="5"/>
-      <c r="W84" s="5"/>
-      <c r="X84" s="5"/>
-      <c r="Y84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+      <c r="T84" s="8"/>
+      <c r="U84" s="8"/>
+      <c r="V84" s="8"/>
+      <c r="W84" s="8"/>
+      <c r="X84" s="8"/>
+      <c r="Y84" s="8"/>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="4"/>
-      <c r="X85" s="4"/>
-      <c r="Y85" s="4"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="8"/>
+      <c r="R85" s="8"/>
+      <c r="S85" s="8"/>
+      <c r="T85" s="8"/>
+      <c r="U85" s="8"/>
+      <c r="V85" s="8"/>
+      <c r="W85" s="8"/>
+      <c r="X85" s="8"/>
+      <c r="Y85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="5"/>
-      <c r="N86" s="5"/>
-      <c r="O86" s="5"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="5"/>
-      <c r="R86" s="5"/>
-      <c r="S86" s="5"/>
-      <c r="T86" s="5"/>
-      <c r="U86" s="5"/>
-      <c r="V86" s="5"/>
-      <c r="W86" s="5"/>
-      <c r="X86" s="5"/>
-      <c r="Y86" s="5"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+      <c r="U86" s="4"/>
+      <c r="V86" s="4"/>
+      <c r="W86" s="4"/>
+      <c r="X86" s="4"/>
+      <c r="Y86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
-      <c r="S87" s="4"/>
-      <c r="T87" s="4"/>
-      <c r="U87" s="4"/>
-      <c r="V87" s="4"/>
-      <c r="W87" s="4"/>
-      <c r="X87" s="4"/>
-      <c r="Y87" s="4"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="8"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="8"/>
+      <c r="Q87" s="8"/>
+      <c r="R87" s="8"/>
+      <c r="S87" s="8"/>
+      <c r="T87" s="8"/>
+      <c r="U87" s="8"/>
+      <c r="V87" s="8"/>
+      <c r="W87" s="8"/>
+      <c r="X87" s="8"/>
+      <c r="Y87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-      <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
-      <c r="R88" s="5"/>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="5"/>
-      <c r="V88" s="5"/>
-      <c r="W88" s="5"/>
-      <c r="X88" s="5"/>
-      <c r="Y88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+      <c r="U88" s="4"/>
+      <c r="V88" s="4"/>
+      <c r="W88" s="4"/>
+      <c r="X88" s="4"/>
+      <c r="Y88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="18"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="19"/>
-      <c r="H89" s="19"/>
-      <c r="I89" s="19"/>
-      <c r="J89" s="19"/>
-      <c r="K89" s="19"/>
-      <c r="L89" s="19"/>
-      <c r="M89" s="19"/>
-      <c r="N89" s="19"/>
-      <c r="O89" s="19"/>
-      <c r="P89" s="19"/>
-      <c r="Q89" s="19"/>
-      <c r="R89" s="19"/>
-      <c r="S89" s="19"/>
-      <c r="T89" s="19"/>
-      <c r="U89" s="19"/>
-      <c r="V89" s="19"/>
-      <c r="W89" s="19"/>
-      <c r="X89" s="19"/>
-      <c r="Y89" s="19"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="8"/>
+      <c r="Q89" s="8"/>
+      <c r="R89" s="8"/>
+      <c r="S89" s="8"/>
+      <c r="T89" s="8"/>
+      <c r="U89" s="8"/>
+      <c r="V89" s="8"/>
+      <c r="W89" s="8"/>
+      <c r="X89" s="8"/>
+      <c r="Y89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="18"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
-      <c r="D90" s="19"/>
+      <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="G90" s="19"/>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
-      <c r="J90" s="19"/>
-      <c r="K90" s="19"/>
-      <c r="L90" s="19"/>
-      <c r="M90" s="19"/>
-      <c r="N90" s="19"/>
-      <c r="O90" s="19"/>
-      <c r="P90" s="19"/>
-      <c r="Q90" s="19"/>
-      <c r="R90" s="19"/>
-      <c r="S90" s="19"/>
-      <c r="T90" s="19"/>
-      <c r="U90" s="19"/>
-      <c r="V90" s="19"/>
-      <c r="W90" s="19"/>
-      <c r="X90" s="19"/>
-      <c r="Y90" s="19"/>
+      <c r="G90" s="22"/>
+      <c r="H90" s="22"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="22"/>
+      <c r="L90" s="22"/>
+      <c r="M90" s="22"/>
+      <c r="N90" s="22"/>
+      <c r="O90" s="22"/>
+      <c r="P90" s="22"/>
+      <c r="Q90" s="22"/>
+      <c r="R90" s="22"/>
+      <c r="S90" s="22"/>
+      <c r="T90" s="22"/>
+      <c r="U90" s="22"/>
+      <c r="V90" s="22"/>
+      <c r="W90" s="22"/>
+      <c r="X90" s="22"/>
+      <c r="Y90" s="22"/>
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="18"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
-      <c r="D91" s="19"/>
+      <c r="D91" s="22"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="G91" s="19"/>
-      <c r="H91" s="19"/>
-      <c r="I91" s="19"/>
-      <c r="J91" s="19"/>
-      <c r="K91" s="19"/>
-      <c r="L91" s="19"/>
-      <c r="M91" s="19"/>
-      <c r="N91" s="19"/>
-      <c r="O91" s="19"/>
-      <c r="P91" s="19"/>
-      <c r="Q91" s="19"/>
-      <c r="R91" s="19"/>
-      <c r="S91" s="19"/>
-      <c r="T91" s="19"/>
-      <c r="U91" s="19"/>
-      <c r="V91" s="19"/>
-      <c r="W91" s="19"/>
-      <c r="X91" s="19"/>
-      <c r="Y91" s="19"/>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="22"/>
+      <c r="L91" s="22"/>
+      <c r="M91" s="22"/>
+      <c r="N91" s="22"/>
+      <c r="O91" s="22"/>
+      <c r="P91" s="22"/>
+      <c r="Q91" s="22"/>
+      <c r="R91" s="22"/>
+      <c r="S91" s="22"/>
+      <c r="T91" s="22"/>
+      <c r="U91" s="22"/>
+      <c r="V91" s="22"/>
+      <c r="W91" s="22"/>
+      <c r="X91" s="22"/>
+      <c r="Y91" s="22"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="21"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="22"/>
+      <c r="N92" s="22"/>
+      <c r="O92" s="22"/>
+      <c r="P92" s="22"/>
+      <c r="Q92" s="22"/>
+      <c r="R92" s="22"/>
+      <c r="S92" s="22"/>
+      <c r="T92" s="22"/>
+      <c r="U92" s="22"/>
+      <c r="V92" s="22"/>
+      <c r="W92" s="22"/>
+      <c r="X92" s="22"/>
+      <c r="Y92" s="22"/>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4296,12 +4373,12 @@
   </sheetData>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1041, "begin group") = COUNTIF($A$1:$A$1041, "end group"))</formula>
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1042, "begin group") = COUNTIF($A$1:$A$1042, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1032, "begin group") = COUNTIF($A$1:$A$1041, "end group")))</formula>
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1033, "begin group") = COUNTIF($A$1:$A$1042, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
@@ -4358,238 +4435,238 @@
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+      <formula>AND($A38="begin group", NOT($B38 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+      <formula>AND($A38="end group", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $L38 = "", $M38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+      <formula>AND($A38="begin repeat", NOT($B38 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+      <formula>AND($A38="end repeat", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $L38 = "", $M38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
-      <formula>AND($I37 = "", $A37 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>AND($I38 = "", $A38 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $B38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+      <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
-      <formula>COUNTIF($B$2:$B$1073,B37)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+      <formula>COUNTIF($B$2:$B$1074,B38)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
+  <conditionalFormatting sqref="A38:Y38">
     <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A38">
     <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+  <conditionalFormatting sqref="E64">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
-      <formula>AND($A63="begin group", NOT($B63 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+      <formula>AND($A64="begin group", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
-      <formula>AND($A63="end group", $B63 = "", $C63 = "", $D63 = "", $E63 = "", $F63 = "", $G63 = "", $H63 = "", $I63 = "", $J63 = "", $K63 = "", $L63 = "", $M63 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+      <formula>AND($A64="end group", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A63="begin repeat", NOT($B63 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+      <formula>AND($A64="begin repeat", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
-      <formula>AND($A63="end repeat", $B63 = "", $C63 = "", $D63 = "", $E63 = "", $F63 = "", $G63 = "", $H63 = "", $I63 = "", $J63 = "", $K63 = "", $L63 = "", $M63 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+      <formula>AND($A64="end repeat", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
     <cfRule type="containsText" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+  <conditionalFormatting sqref="E64">
     <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="A70">
     <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+      <formula>AND($A70="begin group", NOT($B70 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+      <formula>AND($A70="end group", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
     <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="A70">
     <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+      <formula>AND($A70="begin repeat", NOT($B70 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+      <formula>AND($A70="end repeat", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+      <formula>AND($A67="begin group", NOT($B67 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
     <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+      <formula>AND($A67="end group", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
     <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+      <formula>AND($A67="begin repeat", NOT($B67 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
     <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+      <formula>AND($A67="end repeat", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
     <cfRule type="containsText" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
+  <conditionalFormatting sqref="E67">
     <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+  <conditionalFormatting sqref="E69">
     <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
     <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
     <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
     <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
     <cfRule type="containsText" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+  <conditionalFormatting sqref="E69">
     <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I40">
     <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($I35 = "", $A35 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+      <formula>AND($I36 = "", $A36 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
     <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A33="begin group", NOT($B33 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+      <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
     <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
-      <formula>AND($A33="end group", $B33 = "", $C33 = "", $D33 = "", $E33 = "", $F33 = "", $G33 = "", $H33 = "", $I33 = "", $J33 = "", $K33 = "", $L33 = "", $M33 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+      <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
     <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND($A33="begin repeat", NOT($B33 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+      <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
     <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND($A33="end repeat", $B33 = "", $C33 = "", $D33 = "", $E33 = "", $F33 = "", $G33 = "", $H33 = "", $I33 = "", $J33 = "", $K33 = "", $L33 = "", $M33 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36:Y36">
+      <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
     <cfRule type="containsText" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="43"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36:Y36">
+  <conditionalFormatting sqref="A37:Y37">
     <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A37">
     <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($I30 = "", $A30 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+      <formula>AND($I31 = "", $A31 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
     <cfRule type="containsText" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="E37">
     <cfRule type="cellIs" priority="63" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D69 D73:D91" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D12 D14:D70 D74:D92" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D70:D72" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D71:D73" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4614,136 +4691,136 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="1" sqref="13:13 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="B5" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="A6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="A7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="A9" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4767,54 +4844,54 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="13:13 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>164</v>
       </c>
+      <c r="E1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="22" t="n">
+      <c r="A2" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="25" t="n">
         <f aca="true">NOW()</f>
-        <v>44067.7415926847</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" s="11"/>
+        <v>44070.4639687169</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="14"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>